<commit_message>
add progress bar in steps
</commit_message>
<xml_diff>
--- a/server/corelib/lang/all_lang_V1.2.xlsx
+++ b/server/corelib/lang/all_lang_V1.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\digiCenter\server\corelib\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AC82CE6-1491-456C-9C6E-C2F06FE4B8A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF90C70F-7E71-4D11-B2FD-E8FC629CF78D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="724">
   <si>
     <t>name</t>
   </si>
@@ -997,9 +997,6 @@
     <t>Bitte einloggen</t>
   </si>
   <si>
-    <t>(Gast)</t>
-  </si>
-  <si>
     <t>Einstellungen</t>
   </si>
   <si>
@@ -1822,12 +1819,6 @@
   </si>
   <si>
     <t>Wählen Sie das Zeitinterval zum Speichern des Systemprotokolls</t>
-  </si>
-  <si>
-    <t>Temperatur</t>
-  </si>
-  <si>
-    <t>Härte</t>
   </si>
   <si>
     <t>Bitte warten</t>
@@ -2045,6 +2036,356 @@
   <si>
     <t>&lt;h3&gt;請按下&lt;strong&gt; '重試' &lt;/strong&gt;以重測!&lt;/h3&gt;
   &lt;h3&gt;請按下&lt;strong&gt; ' 繼續' &lt;/strong&gt;以量測下一個位置!&lt;/h3&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>head_clicklogin_tooltip</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>click to login</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>點選登入</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Klicken Sie, um sich anzumelden</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqEditor_enable_step</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqEditor_delete_step</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Enable</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delete</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>啟用</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>刪除</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>aktivieren</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>löschen</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>run_load_seq_plhd</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Please load sequence file</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>button-config</t>
+  </si>
+  <si>
+    <t>add_new_role_btn</t>
+  </si>
+  <si>
+    <t>delete_new_role_btn</t>
+  </si>
+  <si>
+    <t>apply_change_user_fnc</t>
+  </si>
+  <si>
+    <t>add_new_user_btn</t>
+  </si>
+  <si>
+    <t>delete_user_btn</t>
+  </si>
+  <si>
+    <t>activate_user_btn</t>
+  </si>
+  <si>
+    <t>deactivate_user_btn</t>
+  </si>
+  <si>
+    <t>new_pw_btn</t>
+  </si>
+  <si>
+    <t>download_syslog_btn</t>
+  </si>
+  <si>
+    <t>button-seqEditor</t>
+  </si>
+  <si>
+    <t>create_seq</t>
+  </si>
+  <si>
+    <t>open_seq</t>
+  </si>
+  <si>
+    <t>save_seq</t>
+  </si>
+  <si>
+    <t>button-run</t>
+  </si>
+  <si>
+    <t>new_a_batch</t>
+  </si>
+  <si>
+    <t>load_a_batch</t>
+  </si>
+  <si>
+    <t>open_test_seq</t>
+  </si>
+  <si>
+    <t>batchConfirm</t>
+  </si>
+  <si>
+    <t>start_test</t>
+  </si>
+  <si>
+    <t>stop_test</t>
+  </si>
+  <si>
+    <t>button-report</t>
+  </si>
+  <si>
+    <t>query-data</t>
+  </si>
+  <si>
+    <t>export-test-data-to-file</t>
+  </si>
+  <si>
+    <t>export-start</t>
+  </si>
+  <si>
+    <t>Configuration Item in Sidebar</t>
+  </si>
+  <si>
+    <t>左列之系統設置</t>
+  </si>
+  <si>
+    <t>Change System Configuration</t>
+  </si>
+  <si>
+    <t>更新系統設定參數</t>
+  </si>
+  <si>
+    <t>Add New User Role</t>
+  </si>
+  <si>
+    <t>新增使用者權限</t>
+  </si>
+  <si>
+    <t>Delete User Role</t>
+  </si>
+  <si>
+    <t>刪除使用者權限</t>
+  </si>
+  <si>
+    <t>Change User Permission</t>
+  </si>
+  <si>
+    <t>更新使用者權限</t>
+  </si>
+  <si>
+    <t>Add New User</t>
+  </si>
+  <si>
+    <t>新增使用者帳號</t>
+  </si>
+  <si>
+    <t>Delete User</t>
+  </si>
+  <si>
+    <t>刪除使用者帳號</t>
+  </si>
+  <si>
+    <t>Activate User</t>
+  </si>
+  <si>
+    <t>啟用使用者帳號</t>
+  </si>
+  <si>
+    <t>Deactivate User</t>
+  </si>
+  <si>
+    <t>停用使用者帳號</t>
+  </si>
+  <si>
+    <t>Provide New Password</t>
+  </si>
+  <si>
+    <t>提供使用者新密碼</t>
+  </si>
+  <si>
+    <t>Download System log</t>
+  </si>
+  <si>
+    <t>下載系統日誌</t>
+  </si>
+  <si>
+    <t>SeqEditor Item in Sidebar</t>
+  </si>
+  <si>
+    <t>Create Sequence</t>
+  </si>
+  <si>
+    <t>Load Sequence</t>
+  </si>
+  <si>
+    <t>Save Sequence</t>
+  </si>
+  <si>
+    <t>Run Item in Sidebar</t>
+  </si>
+  <si>
+    <t>左列之執行測試</t>
+  </si>
+  <si>
+    <t>Create Batch</t>
+  </si>
+  <si>
+    <t>新增批號</t>
+  </si>
+  <si>
+    <t>Load Batch</t>
+  </si>
+  <si>
+    <t>讀取批號</t>
+  </si>
+  <si>
+    <t>Select Test Sequence</t>
+  </si>
+  <si>
+    <t>Confirm Batch Info</t>
+  </si>
+  <si>
+    <t>確認批號資訊</t>
+  </si>
+  <si>
+    <t>Start Test</t>
+  </si>
+  <si>
+    <t>開始測試</t>
+  </si>
+  <si>
+    <t>Stop Test</t>
+  </si>
+  <si>
+    <t>停止測試</t>
+  </si>
+  <si>
+    <t>Report Item in Sidebar</t>
+  </si>
+  <si>
+    <t>左列之報告檢視</t>
+  </si>
+  <si>
+    <t>Query Test Data</t>
+  </si>
+  <si>
+    <t>搜尋測試數據</t>
+  </si>
+  <si>
+    <t>Export Report Option Button</t>
+  </si>
+  <si>
+    <t>呼叫匯出測試數據選單</t>
+  </si>
+  <si>
+    <t>Export data to File Button</t>
+  </si>
+  <si>
+    <t>執行匯出測試數據</t>
+  </si>
+  <si>
+    <t>apply_change_general</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>請讀取測試流程檔案..</t>
+  </si>
+  <si>
+    <t>左列之測試流程編輯</t>
+  </si>
+  <si>
+    <t>新增測試流程</t>
+  </si>
+  <si>
+    <t>讀取測試流程</t>
+  </si>
+  <si>
+    <t>儲存測試流程</t>
+  </si>
+  <si>
+    <t>選擇測試流程</t>
+  </si>
+  <si>
+    <t>Humidity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>濕度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Feuchtigkeit</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>main_indicator_humidity</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>main_indicator_temperature</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>main_indicator_hard</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>硬度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>溫度</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Temperatur</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Temperatur</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Härte</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Härte</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2142,7 +2483,37 @@
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2617,10 +2988,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E169"/>
+  <dimension ref="A1:E202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D86" sqref="D86"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2676,7 +3047,7 @@
         <v>116</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>325</v>
+        <v>621</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2684,16 +3055,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>617</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>223</v>
+        <v>618</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>619</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>326</v>
+        <v>620</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2701,16 +3072,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>610</v>
+        <v>223</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>550</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2718,16 +3089,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>612</v>
+        <v>549</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2735,16 +3106,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>224</v>
+        <v>608</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>120</v>
+        <v>609</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2752,16 +3123,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2769,16 +3140,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>328</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2786,16 +3157,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2803,16 +3174,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>222</v>
+        <v>227</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2820,16 +3191,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2837,16 +3208,16 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2854,16 +3225,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>126</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2871,16 +3242,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>332</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2888,7 +3259,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>127</v>
@@ -2897,7 +3268,7 @@
         <v>231</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2905,16 +3276,16 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2922,7 +3293,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>128</v>
@@ -2931,7 +3302,7 @@
         <v>232</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2939,16 +3310,16 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2956,7 +3327,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>129</v>
@@ -2965,7 +3336,7 @@
         <v>233</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2973,16 +3344,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2990,16 +3361,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3007,16 +3378,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3024,16 +3395,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3041,16 +3412,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3058,16 +3429,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3075,16 +3446,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>413</v>
+        <v>239</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>136</v>
+        <v>339</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3092,16 +3463,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>240</v>
+        <v>412</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3109,16 +3480,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>341</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3126,16 +3497,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>415</v>
+        <v>28</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>417</v>
+        <v>138</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>416</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>551</v>
+        <v>241</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3146,13 +3517,13 @@
         <v>414</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>139</v>
+        <v>416</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>342</v>
+        <v>415</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>550</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3160,16 +3531,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>29</v>
+        <v>413</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3177,16 +3548,16 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3194,16 +3565,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3211,16 +3582,16 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3228,16 +3599,16 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>144</v>
+        <v>345</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3245,16 +3616,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>347</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3262,16 +3633,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3279,16 +3650,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3296,16 +3667,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3313,16 +3684,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -3330,16 +3701,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>333</v>
+        <v>350</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3347,16 +3718,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>352</v>
+        <v>332</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3364,16 +3735,16 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>250</v>
+        <v>254</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3381,16 +3752,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3398,16 +3769,16 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3415,16 +3786,16 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>552</v>
+        <v>352</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3432,16 +3803,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>228</v>
+        <v>256</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>330</v>
+        <v>551</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3449,16 +3820,16 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>257</v>
+        <v>228</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>354</v>
+        <v>329</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3466,16 +3837,16 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3483,16 +3854,16 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -3500,16 +3871,16 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>349</v>
+        <v>355</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -3517,16 +3888,16 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>157</v>
+        <v>348</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -3534,16 +3905,16 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>355</v>
+        <v>157</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -3551,16 +3922,16 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>418</v>
+        <v>51</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>421</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>554</v>
+        <v>155</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -3568,16 +3939,16 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>423</v>
-      </c>
       <c r="D56" s="3" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>327</v>
+        <v>553</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -3585,16 +3956,16 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>553</v>
+        <v>422</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>421</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -3602,16 +3973,16 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>474</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>555</v>
+        <v>424</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>552</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -3619,16 +3990,16 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>556</v>
+        <v>720</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -3636,16 +4007,16 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>557</v>
+        <v>722</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -3653,16 +4024,16 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -3670,16 +4041,16 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -3687,16 +4058,16 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>338</v>
+        <v>556</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -3704,16 +4075,16 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>560</v>
+        <v>337</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -3721,16 +4092,16 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>482</v>
+        <v>466</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -3738,16 +4109,16 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>434</v>
+        <v>622</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="D66" s="4" t="s">
-        <v>483</v>
+        <v>624</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>626</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>562</v>
+        <v>628</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -3755,16 +4126,16 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>435</v>
+        <v>623</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>470</v>
+        <v>625</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>484</v>
+        <v>627</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>563</v>
+        <v>629</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -3772,16 +4143,16 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>469</v>
+        <v>481</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -3789,16 +4160,16 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -3806,16 +4177,16 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>568</v>
+        <v>560</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -3823,16 +4194,16 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -3840,16 +4211,16 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>444</v>
+        <v>470</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -3857,16 +4228,16 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>445</v>
+        <v>471</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>160</v>
+        <v>565</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -3874,16 +4245,16 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>446</v>
+        <v>472</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -3891,16 +4262,16 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>443</v>
+        <v>630</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="D75" s="4" t="s">
-        <v>492</v>
+        <v>631</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>706</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>570</v>
+        <v>632</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -3908,16 +4279,16 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>448</v>
+        <v>439</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>335</v>
+        <v>564</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -3925,16 +4296,16 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>571</v>
+        <v>160</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -3942,16 +4313,16 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>450</v>
+        <v>441</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
@@ -3959,16 +4330,16 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>451</v>
+        <v>442</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
@@ -3976,16 +4347,16 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>454</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>574</v>
+        <v>334</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -3993,16 +4364,16 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>458</v>
+        <v>448</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>575</v>
+        <v>568</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -4010,16 +4381,16 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>459</v>
+        <v>449</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>500</v>
+        <v>456</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>576</v>
+        <v>569</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -4027,16 +4398,16 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>598</v>
+        <v>450</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>599</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>601</v>
+        <v>452</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>495</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -4044,16 +4415,16 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>602</v>
+        <v>451</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>604</v>
+        <v>453</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>606</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>601</v>
+        <v>496</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>571</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -4061,33 +4432,33 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>603</v>
+        <v>457</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>605</v>
+        <v>459</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>607</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+        <v>497</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>85</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>608</v>
-      </c>
-      <c r="C86" s="5" t="s">
-        <v>609</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>619</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>601</v>
+        <v>458</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -4095,16 +4466,16 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>613</v>
+        <v>595</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>615</v>
-      </c>
-      <c r="D87" s="4" t="s">
-        <v>618</v>
+        <v>597</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>596</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -4112,16 +4483,16 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>614</v>
+        <v>599</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>616</v>
+        <v>601</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>617</v>
+        <v>603</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -4129,33 +4500,33 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>261</v>
+        <v>602</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>604</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>89</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>262</v>
+        <v>605</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>616</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>567</v>
+        <v>598</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -4163,16 +4534,16 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>53</v>
+        <v>610</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>263</v>
+        <v>612</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>615</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>160</v>
+        <v>598</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -4180,16 +4551,16 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>54</v>
+        <v>611</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>254</v>
+        <v>613</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>614</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>358</v>
+        <v>598</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -4197,16 +4568,16 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>55</v>
+        <v>594</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -4214,16 +4585,16 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>360</v>
+        <v>564</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -4231,16 +4602,16 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>361</v>
+        <v>160</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -4248,16 +4619,16 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -4265,16 +4636,16 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -4282,16 +4653,16 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>526</v>
+        <v>163</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>527</v>
+        <v>265</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>528</v>
+        <v>359</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -4299,16 +4670,16 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -4316,16 +4687,16 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -4333,16 +4704,16 @@
         <v>100</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
@@ -4350,16 +4721,16 @@
         <v>101</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>170</v>
+        <v>525</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>272</v>
+        <v>526</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>367</v>
+        <v>527</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
@@ -4367,16 +4738,16 @@
         <v>102</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -4384,16 +4755,16 @@
         <v>103</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -4401,16 +4772,16 @@
         <v>104</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -4418,16 +4789,16 @@
         <v>105</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -4435,16 +4806,16 @@
         <v>106</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
@@ -4452,16 +4823,16 @@
         <v>107</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
@@ -4469,16 +4840,16 @@
         <v>108</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -4486,16 +4857,16 @@
         <v>109</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>178</v>
+        <v>370</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -4503,16 +4874,16 @@
         <v>110</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -4520,16 +4891,16 @@
         <v>111</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -4537,16 +4908,16 @@
         <v>112</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -4554,16 +4925,16 @@
         <v>113</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>378</v>
+        <v>178</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -4571,16 +4942,16 @@
         <v>114</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -4588,16 +4959,16 @@
         <v>115</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -4605,16 +4976,16 @@
         <v>116</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -4622,16 +4993,16 @@
         <v>117</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4639,16 +5010,16 @@
         <v>118</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>577</v>
+        <v>378</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
@@ -4656,16 +5027,16 @@
         <v>119</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -4673,16 +5044,16 @@
         <v>120</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -4690,16 +5061,16 @@
         <v>121</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -4707,16 +5078,16 @@
         <v>122</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>386</v>
+        <v>574</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
@@ -4724,16 +5095,16 @@
         <v>123</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
@@ -4741,16 +5112,16 @@
         <v>124</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>388</v>
+        <v>383</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
@@ -4758,16 +5129,16 @@
         <v>125</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -4775,16 +5146,16 @@
         <v>126</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -4792,16 +5163,16 @@
         <v>127</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -4809,16 +5180,16 @@
         <v>128</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -4826,16 +5197,16 @@
         <v>129</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>393</v>
+        <v>388</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -4843,16 +5214,16 @@
         <v>130</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>394</v>
+        <v>389</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -4860,16 +5231,16 @@
         <v>131</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>578</v>
+        <v>390</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -4877,16 +5248,16 @@
         <v>132</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -4894,16 +5265,16 @@
         <v>133</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -4911,16 +5282,16 @@
         <v>134</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -4928,16 +5299,16 @@
         <v>135</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>398</v>
+        <v>575</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -4945,16 +5316,16 @@
         <v>136</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -4962,16 +5333,16 @@
         <v>137</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -4979,16 +5350,16 @@
         <v>138</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -4996,16 +5367,16 @@
         <v>139</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -5013,16 +5384,16 @@
         <v>140</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -5030,16 +5401,16 @@
         <v>141</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>531</v>
+        <v>100</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
@@ -5047,16 +5418,16 @@
         <v>142</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>533</v>
+        <v>101</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>534</v>
+        <v>207</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>535</v>
-      </c>
-      <c r="E143" s="3" t="s">
-        <v>579</v>
+        <v>309</v>
+      </c>
+      <c r="E143" s="1" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
@@ -5064,16 +5435,16 @@
         <v>143</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>532</v>
+        <v>102</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>529</v>
+        <v>208</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="E144" s="3" t="s">
-        <v>580</v>
+        <v>310</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>401</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -5081,16 +5452,16 @@
         <v>144</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>536</v>
+        <v>103</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>537</v>
+        <v>209</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>538</v>
-      </c>
-      <c r="E145" s="3" t="s">
-        <v>581</v>
+        <v>311</v>
+      </c>
+      <c r="E145" s="1" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
@@ -5098,16 +5469,16 @@
         <v>145</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>104</v>
+        <v>530</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
@@ -5115,16 +5486,16 @@
         <v>146</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>105</v>
+        <v>532</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>212</v>
+        <v>533</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>406</v>
+        <v>534</v>
+      </c>
+      <c r="E147" s="3" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
@@ -5132,16 +5503,16 @@
         <v>147</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>106</v>
+        <v>531</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>213</v>
+        <v>528</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="E148" s="1" t="s">
-        <v>407</v>
+        <v>529</v>
+      </c>
+      <c r="E148" s="3" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
@@ -5149,16 +5520,16 @@
         <v>148</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>107</v>
+        <v>535</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>214</v>
+        <v>536</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="E149" s="1" t="s">
-        <v>408</v>
+        <v>537</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
@@ -5166,16 +5537,16 @@
         <v>149</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="E150" s="1" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
@@ -5183,16 +5554,16 @@
         <v>150</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="E151" s="1" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
@@ -5200,16 +5571,16 @@
         <v>151</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
@@ -5217,16 +5588,16 @@
         <v>152</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -5234,16 +5605,16 @@
         <v>153</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>219</v>
+        <v>408</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -5251,16 +5622,16 @@
         <v>154</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>220</v>
+        <v>409</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -5268,16 +5639,16 @@
         <v>155</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>502</v>
+        <v>110</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>503</v>
-      </c>
-      <c r="D156" s="4" t="s">
-        <v>504</v>
-      </c>
-      <c r="E156" s="4" t="s">
-        <v>582</v>
+        <v>217</v>
+      </c>
+      <c r="D156" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
@@ -5285,84 +5656,84 @@
         <v>156</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>505</v>
+        <v>111</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>506</v>
-      </c>
-      <c r="D157" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="E157" s="4" t="s">
-        <v>583</v>
+        <v>218</v>
+      </c>
+      <c r="D157" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="E157" s="1" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
         <v>157</v>
       </c>
-      <c r="B158" s="3" t="s">
-        <v>515</v>
+      <c r="B158" s="1" t="s">
+        <v>112</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>508</v>
+        <v>219</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>509</v>
+        <v>321</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>584</v>
+        <v>219</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
         <v>158</v>
       </c>
-      <c r="B159" s="3" t="s">
-        <v>516</v>
+      <c r="B159" s="1" t="s">
+        <v>113</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>514</v>
+        <v>220</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>518</v>
+        <v>322</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>585</v>
+        <v>220</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
         <v>159</v>
       </c>
-      <c r="B160" s="3" t="s">
-        <v>512</v>
+      <c r="B160" s="1" t="s">
+        <v>501</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="D160" s="1" t="s">
-        <v>511</v>
-      </c>
-      <c r="E160" s="1" t="s">
-        <v>586</v>
+        <v>502</v>
+      </c>
+      <c r="D160" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="E160" s="4" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
         <v>160</v>
       </c>
-      <c r="B161" s="3" t="s">
-        <v>513</v>
+      <c r="B161" s="1" t="s">
+        <v>504</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="D161" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="E161" s="1" t="s">
-        <v>587</v>
+        <v>505</v>
+      </c>
+      <c r="D161" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="E161" s="4" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
@@ -5370,16 +5741,16 @@
         <v>161</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>520</v>
+        <v>514</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>522</v>
+        <v>507</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
       <c r="E162" s="1" t="s">
-        <v>588</v>
+        <v>581</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
@@ -5387,16 +5758,16 @@
         <v>162</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>521</v>
+        <v>515</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>525</v>
+        <v>517</v>
       </c>
       <c r="E163" s="1" t="s">
-        <v>589</v>
+        <v>582</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
@@ -5404,16 +5775,16 @@
         <v>163</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>539</v>
+        <v>511</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>541</v>
+        <v>509</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>542</v>
+        <v>510</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>590</v>
+        <v>583</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
@@ -5421,16 +5792,16 @@
         <v>164</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>540</v>
+        <v>512</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>596</v>
+        <v>516</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>543</v>
+        <v>518</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>595</v>
+        <v>584</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
@@ -5438,16 +5809,16 @@
         <v>165</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>544</v>
+        <v>519</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>547</v>
+        <v>521</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>546</v>
+        <v>523</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
@@ -5455,16 +5826,16 @@
         <v>166</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>545</v>
+        <v>520</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>596</v>
+        <v>522</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>543</v>
+        <v>524</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>595</v>
+        <v>586</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
@@ -5472,16 +5843,16 @@
         <v>167</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>594</v>
-      </c>
-      <c r="D168" s="6" t="s">
-        <v>592</v>
+        <v>540</v>
+      </c>
+      <c r="D168" s="1" t="s">
+        <v>541</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
@@ -5489,86 +5860,662 @@
         <v>168</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D169" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
+        <v>169</v>
+      </c>
+      <c r="B170" s="3" t="s">
         <v>543</v>
       </c>
-      <c r="E169" s="1" t="s">
-        <v>595</v>
+      <c r="C170" s="1" t="s">
+        <v>546</v>
+      </c>
+      <c r="D170" s="1" t="s">
+        <v>545</v>
+      </c>
+      <c r="E170" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
+        <v>170</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="D171" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="E171" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
+        <v>171</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="C172" s="1" t="s">
+        <v>591</v>
+      </c>
+      <c r="D172" s="6" t="s">
+        <v>589</v>
+      </c>
+      <c r="E172" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
+        <v>172</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="C173" s="1" t="s">
+        <v>593</v>
+      </c>
+      <c r="D173" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="E173" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
+        <v>173</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="C174" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="D174" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="E174" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
+        <v>174</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>705</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>660</v>
+      </c>
+      <c r="D175" s="1" t="s">
+        <v>661</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
+        <v>175</v>
+      </c>
+      <c r="B176" s="1" t="s">
+        <v>634</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>662</v>
+      </c>
+      <c r="D176" s="1" t="s">
+        <v>663</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A177" s="2">
+        <v>176</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="D177" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A178" s="2">
+        <v>177</v>
+      </c>
+      <c r="B178" s="1" t="s">
+        <v>636</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="D178" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A179" s="2">
+        <v>178</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>637</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="D179" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A180" s="2">
+        <v>179</v>
+      </c>
+      <c r="B180" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="D180" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A181" s="2">
+        <v>180</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>639</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>672</v>
+      </c>
+      <c r="D181" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A182" s="2">
+        <v>181</v>
+      </c>
+      <c r="B182" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="D182" s="1" t="s">
+        <v>675</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A183" s="2">
+        <v>182</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="D183" s="1" t="s">
+        <v>677</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A184" s="2">
+        <v>183</v>
+      </c>
+      <c r="B184" s="1" t="s">
+        <v>642</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="D184" s="1" t="s">
+        <v>679</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A185" s="2">
+        <v>184</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>680</v>
+      </c>
+      <c r="D185" s="1" t="s">
+        <v>707</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A186" s="2">
+        <v>185</v>
+      </c>
+      <c r="B186" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>681</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>708</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A187" s="2">
+        <v>186</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>682</v>
+      </c>
+      <c r="D187" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A188" s="2">
+        <v>187</v>
+      </c>
+      <c r="B188" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="D188" s="1" t="s">
+        <v>710</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A189" s="2">
+        <v>188</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="D189" s="1" t="s">
+        <v>685</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
+        <v>189</v>
+      </c>
+      <c r="B190" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>686</v>
+      </c>
+      <c r="D190" s="1" t="s">
+        <v>687</v>
+      </c>
+      <c r="E190" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A191" s="2">
+        <v>190</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="D191" s="1" t="s">
+        <v>689</v>
+      </c>
+      <c r="E191" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A192" s="2">
+        <v>191</v>
+      </c>
+      <c r="B192" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>690</v>
+      </c>
+      <c r="D192" s="1" t="s">
+        <v>711</v>
+      </c>
+      <c r="E192" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="2">
+        <v>192</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>651</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="D193" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="E193" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
+        <v>193</v>
+      </c>
+      <c r="B194" s="1" t="s">
+        <v>652</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>693</v>
+      </c>
+      <c r="D194" s="1" t="s">
+        <v>694</v>
+      </c>
+      <c r="E194" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="2">
+        <v>194</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>653</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>695</v>
+      </c>
+      <c r="D195" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="E195" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="2">
+        <v>195</v>
+      </c>
+      <c r="B196" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="E196" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
+        <v>196</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>699</v>
+      </c>
+      <c r="D197" s="1" t="s">
+        <v>700</v>
+      </c>
+      <c r="E197" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
+        <v>197</v>
+      </c>
+      <c r="B198" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="C198" s="1" t="s">
+        <v>701</v>
+      </c>
+      <c r="D198" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="E198" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="2">
+        <v>198</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="C199" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="D199" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="E199" s="1" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="2">
+        <v>199</v>
+      </c>
+      <c r="B200" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="C200" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D200" s="4" t="s">
+        <v>718</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="2">
+        <v>200</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="C201" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="D201" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="E201" s="3" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="2">
+        <v>201</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>712</v>
+      </c>
+      <c r="D202" s="4" t="s">
+        <v>713</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>714</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B160:E161 B170:E1048576 B1:E82 B146:E158 B89:E144">
+  <conditionalFormatting sqref="B164:E165 B1:E3 B150:E162 B93:E148 B68:E86 B5:E65 B174:E199 B202:E1048576">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B163:E163">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B166:E167">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B149:E149">
     <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B159:E159">
+  <conditionalFormatting sqref="B168:E168 B169 D169:E169">
     <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B162:E163">
+  <conditionalFormatting sqref="B170:E170 B171 D171:E171">
     <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B145:E145">
+  <conditionalFormatting sqref="B172:E173">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B164:E164 B165 D165:E165">
+  <conditionalFormatting sqref="C171">
     <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B166:E166 B167 D167:E167">
+  <conditionalFormatting sqref="C169">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B168:E169">
+  <conditionalFormatting sqref="B87:E87">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C167">
+  <conditionalFormatting sqref="B88:D90">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C165">
+  <conditionalFormatting sqref="E88:E90">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B83:E83">
+  <conditionalFormatting sqref="B91:D92">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B84:D86">
+  <conditionalFormatting sqref="E91:E92">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E84:E86">
+  <conditionalFormatting sqref="B4:E4">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B87:D88">
+  <conditionalFormatting sqref="B66:E67">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E87:E88">
+  <conditionalFormatting sqref="B200:E201">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>

</xml_diff>

<commit_message>
add audit trail function in user management and seq saving improve save log function
</commit_message>
<xml_diff>
--- a/server/corelib/lang/all_lang_V1.2.xlsx
+++ b/server/corelib/lang/all_lang_V1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\digiCenter\server\corelib\lang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF90C70F-7E71-4D11-B2FD-E8FC629CF78D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D19E3184-D65A-4C2A-BA5A-C1E66AF95CC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-57720" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="730">
   <si>
     <t>name</t>
   </si>
@@ -2386,6 +2386,32 @@
   </si>
   <si>
     <t>Härte</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqEditor_inform_seq_differ_title</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>seqEditor_inform_seq_differ_txt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>測試流程已更動</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sequence are changed!</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>測試流程內容已被更動，是否更新?
+########## 更動內容 ##########</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Content of selected sequence are changed! Apply changes?
+########## Detail of changes ##########</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2459,7 +2485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2479,11 +2505,44 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2988,10 +3047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E202"/>
+  <dimension ref="A1:E204"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A202"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4208,322 +4267,322 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>436</v>
+        <v>724</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="D72" s="4" t="s">
-        <v>485</v>
+        <v>727</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>726</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>562</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>486</v>
+        <v>725</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>729</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>728</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>565</v>
+        <v>598</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>630</v>
+        <v>437</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>706</v>
+        <v>471</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>486</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>632</v>
+        <v>565</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>443</v>
+        <v>472</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>440</v>
+        <v>630</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>444</v>
-      </c>
-      <c r="D77" s="4" t="s">
-        <v>489</v>
+        <v>631</v>
+      </c>
+      <c r="D77" s="6" t="s">
+        <v>706</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>160</v>
+        <v>632</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>567</v>
+        <v>160</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>454</v>
+        <v>445</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>334</v>
+        <v>566</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>455</v>
+        <v>446</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>569</v>
+        <v>334</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="D85" s="4" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>499</v>
+        <v>453</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>595</v>
+        <v>457</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>597</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>596</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>598</v>
+        <v>459</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>497</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>572</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>599</v>
+        <v>458</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>601</v>
+        <v>499</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>598</v>
+        <v>498</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>573</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>602</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>604</v>
+        <v>597</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>596</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>605</v>
-      </c>
-      <c r="C90" s="5" t="s">
-        <v>606</v>
-      </c>
-      <c r="D90" s="5" t="s">
-        <v>616</v>
+        <v>599</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>601</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>603</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>598</v>
@@ -4531,33 +4590,33 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>610</v>
+        <v>600</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>612</v>
+        <v>602</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>613</v>
-      </c>
-      <c r="D92" s="4" t="s">
-        <v>614</v>
+        <v>605</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="D92" s="5" t="s">
+        <v>616</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>598</v>
@@ -4565,1336 +4624,1336 @@
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>594</v>
+        <v>610</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>261</v>
+        <v>612</v>
+      </c>
+      <c r="D93" s="4" t="s">
+        <v>615</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>356</v>
+        <v>598</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>52</v>
+        <v>611</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>262</v>
+        <v>613</v>
+      </c>
+      <c r="D94" s="4" t="s">
+        <v>614</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>564</v>
+        <v>598</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>53</v>
+        <v>594</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>160</v>
+        <v>356</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>254</v>
+        <v>262</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>357</v>
+        <v>564</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>358</v>
+        <v>160</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>525</v>
+        <v>165</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>526</v>
+        <v>267</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>527</v>
+        <v>361</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="2">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>168</v>
+        <v>525</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>270</v>
+        <v>526</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>364</v>
+        <v>527</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="2">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="2">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="2">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="2">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="2">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="2">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="2">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>178</v>
+        <v>372</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="2">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="2">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>375</v>
+        <v>178</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="2">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="2">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="E118" s="1" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" s="2">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E119" s="1" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="2">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E120" s="1" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="2">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E121" s="1" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="2">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>574</v>
+        <v>380</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="2">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="2">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>383</v>
+        <v>574</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="2">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E126" s="1" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="2">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="2">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E128" s="1" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="2">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="E129" s="1" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="2">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E130" s="1" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="2">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="E131" s="1" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="2">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E132" s="1" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="2">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E133" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="2">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E134" s="1" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="2">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E135" s="1" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="2">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E136" s="1" t="s">
-        <v>575</v>
+        <v>392</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="2">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E137" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E138" s="1" t="s">
-        <v>395</v>
+        <v>575</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="2">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E139" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="2">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="E140" s="1" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="2">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E141" s="1" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="2">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="E142" s="1" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="2">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E143" s="1" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="2">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="E144" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="2">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="E145" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>530</v>
+        <v>102</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E146" s="1" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="2">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>532</v>
+        <v>103</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>533</v>
+        <v>209</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>534</v>
-      </c>
-      <c r="E147" s="3" t="s">
-        <v>576</v>
+        <v>311</v>
+      </c>
+      <c r="E147" s="1" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="2">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>528</v>
+        <v>210</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="E148" s="3" t="s">
-        <v>577</v>
+        <v>312</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>403</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="2">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="E149" s="3" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="2">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>104</v>
+        <v>531</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>211</v>
+        <v>528</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>404</v>
+        <v>529</v>
+      </c>
+      <c r="E150" s="3" t="s">
+        <v>577</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="2">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>105</v>
+        <v>535</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>212</v>
+        <v>536</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>405</v>
+        <v>537</v>
+      </c>
+      <c r="E151" s="3" t="s">
+        <v>578</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="2">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B152" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E152" s="1" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" s="2">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B153" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E153" s="1" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" s="2">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B154" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E154" s="1" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" s="2">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B155" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E155" s="1" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" s="2">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="E156" s="1" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" s="2">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B157" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C157" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E157" s="1" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" s="2">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B158" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C158" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E158" s="1" t="s">
-        <v>219</v>
+        <v>410</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" s="2">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B159" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E159" s="1" t="s">
-        <v>220</v>
+        <v>411</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" s="2">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B160" s="1" t="s">
-        <v>501</v>
+        <v>112</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>502</v>
-      </c>
-      <c r="D160" s="4" t="s">
-        <v>503</v>
-      </c>
-      <c r="E160" s="4" t="s">
-        <v>579</v>
+        <v>219</v>
+      </c>
+      <c r="D160" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E160" s="1" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" s="2">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B161" s="1" t="s">
-        <v>504</v>
+        <v>113</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>505</v>
-      </c>
-      <c r="D161" s="4" t="s">
-        <v>506</v>
-      </c>
-      <c r="E161" s="4" t="s">
-        <v>580</v>
+        <v>220</v>
+      </c>
+      <c r="D161" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="E161" s="1" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" s="2">
-        <v>161</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>514</v>
+        <v>159</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>501</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>507</v>
-      </c>
-      <c r="D162" s="1" t="s">
-        <v>508</v>
-      </c>
-      <c r="E162" s="1" t="s">
-        <v>581</v>
+        <v>502</v>
+      </c>
+      <c r="D162" s="4" t="s">
+        <v>503</v>
+      </c>
+      <c r="E162" s="4" t="s">
+        <v>579</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" s="2">
-        <v>162</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>515</v>
+        <v>160</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>504</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="D163" s="1" t="s">
-        <v>517</v>
-      </c>
-      <c r="E163" s="1" t="s">
-        <v>582</v>
+        <v>505</v>
+      </c>
+      <c r="D163" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="E163" s="4" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" s="2">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="E164" s="1" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" s="2">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E165" s="1" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" s="2">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>519</v>
+        <v>511</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>521</v>
+        <v>509</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>523</v>
+        <v>510</v>
       </c>
       <c r="E166" s="1" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" s="2">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>520</v>
+        <v>512</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>524</v>
+        <v>518</v>
       </c>
       <c r="E167" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" s="2">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>538</v>
+        <v>519</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>540</v>
+        <v>521</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>541</v>
+        <v>523</v>
       </c>
       <c r="E168" s="1" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" s="2">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>539</v>
+        <v>520</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>593</v>
+        <v>522</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>542</v>
+        <v>524</v>
       </c>
       <c r="E169" s="1" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>543</v>
+        <v>538</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="E170" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" s="2">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>544</v>
+        <v>539</v>
       </c>
       <c r="C171" s="1" t="s">
         <v>593</v>
@@ -5908,27 +5967,27 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" s="2">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>591</v>
-      </c>
-      <c r="D172" s="6" t="s">
-        <v>589</v>
+        <v>546</v>
+      </c>
+      <c r="D172" s="1" t="s">
+        <v>545</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" s="2">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="C173" s="1" t="s">
         <v>593</v>
@@ -5942,50 +6001,50 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" s="2">
-        <v>173</v>
-      </c>
-      <c r="B174" s="1" t="s">
-        <v>633</v>
+        <v>171</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>547</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="D174" s="1" t="s">
-        <v>659</v>
+        <v>591</v>
+      </c>
+      <c r="D174" s="6" t="s">
+        <v>589</v>
       </c>
       <c r="E174" s="1" t="s">
-        <v>632</v>
+        <v>590</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" s="2">
-        <v>174</v>
-      </c>
-      <c r="B175" s="1" t="s">
-        <v>705</v>
+        <v>172</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>548</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>660</v>
+        <v>593</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>661</v>
+        <v>542</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>632</v>
+        <v>592</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" s="2">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B176" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="E176" s="1" t="s">
         <v>632</v>
@@ -5993,16 +6052,16 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="2">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>635</v>
+        <v>705</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="E177" s="1" t="s">
         <v>632</v>
@@ -6010,16 +6069,16 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="E178" s="1" t="s">
         <v>632</v>
@@ -6027,16 +6086,16 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="2">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="E179" s="1" t="s">
         <v>632</v>
@@ -6044,16 +6103,16 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="2">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B180" s="1" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="E180" s="1" t="s">
         <v>632</v>
@@ -6061,16 +6120,16 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="2">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>632</v>
@@ -6078,16 +6137,16 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="2">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="E182" s="1" t="s">
         <v>632</v>
@@ -6095,16 +6154,16 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="2">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="E183" s="1" t="s">
         <v>632</v>
@@ -6112,16 +6171,16 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="2">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="E184" s="1" t="s">
         <v>632</v>
@@ -6129,16 +6188,16 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="2">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>707</v>
+        <v>677</v>
       </c>
       <c r="E185" s="1" t="s">
         <v>632</v>
@@ -6146,16 +6205,16 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>681</v>
+        <v>678</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>708</v>
+        <v>679</v>
       </c>
       <c r="E186" s="1" t="s">
         <v>632</v>
@@ -6163,16 +6222,16 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="2">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B187" s="1" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="E187" s="1" t="s">
         <v>632</v>
@@ -6180,16 +6239,16 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="2">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="E188" s="1" t="s">
         <v>632</v>
@@ -6197,16 +6256,16 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="2">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>685</v>
+        <v>709</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>632</v>
@@ -6214,16 +6273,16 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="2">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>687</v>
+        <v>710</v>
       </c>
       <c r="E190" s="1" t="s">
         <v>632</v>
@@ -6231,16 +6290,16 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="2">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="E191" s="1" t="s">
         <v>632</v>
@@ -6248,16 +6307,16 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="2">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>711</v>
+        <v>687</v>
       </c>
       <c r="E192" s="1" t="s">
         <v>632</v>
@@ -6265,16 +6324,16 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="2">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="E193" s="1" t="s">
         <v>632</v>
@@ -6282,16 +6341,16 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>694</v>
+        <v>711</v>
       </c>
       <c r="E194" s="1" t="s">
         <v>632</v>
@@ -6299,16 +6358,16 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="2">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="E195" s="1" t="s">
         <v>632</v>
@@ -6316,16 +6375,16 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="2">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="E196" s="1" t="s">
         <v>632</v>
@@ -6333,16 +6392,16 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" s="2">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="E197" s="1" t="s">
         <v>632</v>
@@ -6350,16 +6409,16 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" s="2">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="E198" s="1" t="s">
         <v>632</v>
@@ -6367,16 +6426,16 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" s="2">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="E199" s="1" t="s">
         <v>632</v>
@@ -6384,138 +6443,187 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" s="2">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>717</v>
+        <v>656</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="D200" s="4" t="s">
-        <v>718</v>
-      </c>
-      <c r="E200" s="3" t="s">
-        <v>723</v>
+        <v>701</v>
+      </c>
+      <c r="D200" s="1" t="s">
+        <v>702</v>
+      </c>
+      <c r="E200" s="1" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" s="2">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>716</v>
+        <v>657</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="D201" s="4" t="s">
-        <v>719</v>
-      </c>
-      <c r="E201" s="3" t="s">
-        <v>721</v>
+        <v>703</v>
+      </c>
+      <c r="D201" s="1" t="s">
+        <v>704</v>
+      </c>
+      <c r="E201" s="1" t="s">
+        <v>632</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
+        <v>199</v>
+      </c>
+      <c r="B202" s="1" t="s">
+        <v>717</v>
+      </c>
+      <c r="C202" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D202" s="4" t="s">
+        <v>718</v>
+      </c>
+      <c r="E202" s="3" t="s">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="2">
+        <v>200</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>716</v>
+      </c>
+      <c r="C203" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="D203" s="4" t="s">
+        <v>719</v>
+      </c>
+      <c r="E203" s="3" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="2">
         <v>201</v>
       </c>
-      <c r="B202" s="1" t="s">
+      <c r="B204" s="1" t="s">
         <v>715</v>
       </c>
-      <c r="C202" s="1" t="s">
+      <c r="C204" s="1" t="s">
         <v>712</v>
       </c>
-      <c r="D202" s="4" t="s">
+      <c r="D204" s="4" t="s">
         <v>713</v>
       </c>
-      <c r="E202" s="3" t="s">
+      <c r="E204" s="3" t="s">
         <v>714</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="B164:E165 B1:E3 B150:E162 B93:E148 B68:E86 B5:E65 B174:E199 B202:E1048576">
+  <conditionalFormatting sqref="B166:E167 B1:E3 B152:E164 B95:E150 B68:E71 B5:E65 B176:E201 B204:E1048576 B74:E88">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B165:E165">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B168:E169">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
+      <formula>"TBD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B151:E151">
     <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B163:E163">
+  <conditionalFormatting sqref="B170:E170 B171 D171:E171">
     <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B166:E167">
+  <conditionalFormatting sqref="B172:E172 B173 D173:E173">
     <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B149:E149">
+  <conditionalFormatting sqref="B174:E175">
     <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B168:E168 B169 D169:E169">
+  <conditionalFormatting sqref="C173">
     <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B170:E170 B171 D171:E171">
+  <conditionalFormatting sqref="C171">
     <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B172:E173">
+  <conditionalFormatting sqref="B89:E89">
     <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C171">
+  <conditionalFormatting sqref="B90:D92">
     <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C169">
+  <conditionalFormatting sqref="E90:E92">
     <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B87:E87">
+  <conditionalFormatting sqref="B93:D94">
     <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B88:D90">
+  <conditionalFormatting sqref="E93:E94">
     <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E88:E90">
+  <conditionalFormatting sqref="B4:E4">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B91:D92">
+  <conditionalFormatting sqref="B66:E67">
     <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E91:E92">
+  <conditionalFormatting sqref="B202:E203">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:E4">
+  <conditionalFormatting sqref="B72:D73">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B66:E67">
+  <conditionalFormatting sqref="E73">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B200:E201">
+  <conditionalFormatting sqref="E72">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>

</xml_diff>